<commit_message>
ORGANIZANDO OS MÉTODOS DE MACHINE LEARNING
</commit_message>
<xml_diff>
--- a/dados/Exercicio_estimativa_de_paginas_2019_2020.xlsx
+++ b/dados/Exercicio_estimativa_de_paginas_2019_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2C21A2-F372-6E48-80CF-0B8C3C5F731A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29000F93-F358-C549-B24B-DDBC361E0528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2260" windowWidth="31440" windowHeight="15560" xr2:uid="{65A40DB1-9662-402A-9A88-8271FB79FF7C}"/>
+    <workbookView xWindow="-35900" yWindow="1840" windowWidth="31440" windowHeight="15560" xr2:uid="{65A40DB1-9662-402A-9A88-8271FB79FF7C}"/>
   </bookViews>
   <sheets>
     <sheet name="EXECUTADO 2019" sheetId="4" r:id="rId1"/>
@@ -3052,7 +3052,7 @@
   <dimension ref="A1:Z78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8849,8 +8849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B00B66-C32D-4DEF-9BC0-D9C09304FF24}">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView topLeftCell="S24" workbookViewId="0">
-      <selection activeCell="AB41" sqref="AB41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8862,16 +8862,16 @@
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="102.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="102.6640625" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="6.83203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="7.1640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="8" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="7.1640625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="5.33203125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="11" max="12" width="6.83203125" customWidth="1"/>
+    <col min="13" max="13" width="7.1640625" customWidth="1"/>
+    <col min="14" max="14" width="8" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" customWidth="1"/>
+    <col min="17" max="17" width="7.5" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" customWidth="1"/>
     <col min="19" max="19" width="9" customWidth="1"/>
     <col min="20" max="20" width="20.5" customWidth="1"/>
     <col min="21" max="21" width="23.33203125" customWidth="1"/>

</xml_diff>

<commit_message>
testando modelo - com  arquivos sem nota fiscal
</commit_message>
<xml_diff>
--- a/dados/Exercicio_estimativa_de_paginas_2019_2020.xlsx
+++ b/dados/Exercicio_estimativa_de_paginas_2019_2020.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09368988-159E-6346-9D52-8EE35610A3C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D007CFCA-FCEA-4E49-94F5-BEBABC67BC02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38080" yWindow="780" windowWidth="37280" windowHeight="20140" xr2:uid="{65A40DB1-9662-402A-9A88-8271FB79FF7C}"/>
+    <workbookView xWindow="-38080" yWindow="780" windowWidth="37280" windowHeight="20140" activeTab="4" xr2:uid="{65A40DB1-9662-402A-9A88-8271FB79FF7C}"/>
   </bookViews>
   <sheets>
     <sheet name="EXECUTADO 2019" sheetId="4" r:id="rId1"/>
     <sheet name="EXECUTADO 2020" sheetId="3" r:id="rId2"/>
     <sheet name="EXECUTADO" sheetId="1" state="hidden" r:id="rId3"/>
     <sheet name="EXERCÍCIO" sheetId="2" r:id="rId4"/>
-    <sheet name="SEM NOTA FISCAL" sheetId="5" r:id="rId5"/>
+    <sheet name="SEM_NOTA_FISCAL" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'EXECUTADO 2020'!$A$1:$Z$43</definedName>
@@ -3614,7 +3614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B51CFDF2-E479-4AF3-B196-4948E99A1239}">
   <dimension ref="A1:AB78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
@@ -10003,8 +10003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B00B66-C32D-4DEF-9BC0-D9C09304FF24}">
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22407,8 +22407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164BC1EC-4B9C-FB49-BFE1-CD35C07DC9F3}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>